<commit_message>
Pulling AHS 2013 data and performing MLR using income ~ vintage + size.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw_10_measures.xlsx
+++ b/projects/resstock_pnw_10_measures.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="444">
   <si>
     <t>type</t>
   </si>
@@ -1233,9 +1233,6 @@
     <t>R-10 Crawlspace Walls</t>
   </si>
   <si>
-    <t>R-5 Slab Perimeter</t>
-  </si>
-  <si>
     <t>EnergyStar Dishwashers</t>
   </si>
   <si>
@@ -1363,6 +1360,12 @@
   </si>
   <si>
     <t>Conditioned Floor Area (ft^2)</t>
+  </si>
+  <si>
+    <t>Insulation Unfinished Basement|Wall R-10</t>
+  </si>
+  <si>
+    <t>R-10 Slab Perimeter</t>
   </si>
 </sst>
 </file>
@@ -3592,11 +3595,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1544">
     <cellStyle name="20% - Accent1" xfId="1521" builtinId="30" customBuiltin="1"/>
@@ -5948,7 +5951,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6003,14 +6008,14 @@
       <c r="R1" s="30"/>
       <c r="S1" s="27"/>
       <c r="T1" s="27"/>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
     </row>
     <row r="2" spans="1:26" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
@@ -6426,8 +6431,8 @@
         <v>233</v>
       </c>
       <c r="H11" s="10"/>
-      <c r="I11" s="53" t="s">
-        <v>405</v>
+      <c r="I11" s="52" t="s">
+        <v>404</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
@@ -6465,8 +6470,8 @@
         <v>233</v>
       </c>
       <c r="H12" s="10"/>
-      <c r="I12" s="53" t="s">
-        <v>406</v>
+      <c r="I12" s="52" t="s">
+        <v>405</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -6544,7 +6549,7 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -6654,8 +6659,8 @@
         <v>233</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="53" t="s">
-        <v>405</v>
+      <c r="I17" s="52" t="s">
+        <v>442</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
@@ -6693,8 +6698,8 @@
         <v>233</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="53" t="s">
-        <v>407</v>
+      <c r="I18" s="52" t="s">
+        <v>406</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -6772,7 +6777,7 @@
       </c>
       <c r="H20" s="10"/>
       <c r="I20" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -6882,8 +6887,8 @@
         <v>233</v>
       </c>
       <c r="H23" s="10"/>
-      <c r="I23" s="54" t="s">
-        <v>408</v>
+      <c r="I23" s="53" t="s">
+        <v>407</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -6921,8 +6926,8 @@
         <v>233</v>
       </c>
       <c r="H24" s="10"/>
-      <c r="I24" s="54" t="s">
-        <v>409</v>
+      <c r="I24" s="53" t="s">
+        <v>408</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -7000,7 +7005,7 @@
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -7025,7 +7030,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="48" t="s">
-        <v>399</v>
+        <v>443</v>
       </c>
       <c r="C27" s="48" t="s">
         <v>269</v>
@@ -7062,7 +7067,7 @@
       </c>
       <c r="D28" s="49" t="str">
         <f>"Run " &amp; B27</f>
-        <v>Run R-5 Slab Perimeter</v>
+        <v>Run R-10 Slab Perimeter</v>
       </c>
       <c r="E28" s="49" t="s">
         <v>266</v>
@@ -7111,7 +7116,7 @@
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -7150,7 +7155,7 @@
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7188,7 +7193,9 @@
         <v>169</v>
       </c>
       <c r="H31" s="10"/>
-      <c r="I31" s="51"/>
+      <c r="I31" s="51">
+        <v>1.53</v>
+      </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
@@ -7226,7 +7233,7 @@
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
@@ -7604,7 +7611,7 @@
       </c>
       <c r="H42" s="10"/>
       <c r="I42" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -7642,7 +7649,9 @@
         <v>169</v>
       </c>
       <c r="H43" s="10"/>
-      <c r="I43" s="51"/>
+      <c r="I43" s="51">
+        <v>1.02</v>
+      </c>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
       <c r="L43" s="10"/>
@@ -7791,7 +7800,7 @@
       </c>
       <c r="H47" s="10"/>
       <c r="I47" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
@@ -8017,7 +8026,7 @@
       </c>
       <c r="H53" s="10"/>
       <c r="I53" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
@@ -8157,7 +8166,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="48" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C57" s="48" t="s">
         <v>269</v>
@@ -8224,7 +8233,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="59" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10"/>
       <c r="B59" s="10" t="s">
         <v>20</v>
@@ -8243,7 +8252,7 @@
       </c>
       <c r="H59" s="10"/>
       <c r="I59" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J59" s="10"/>
       <c r="K59" s="10"/>
@@ -8263,7 +8272,7 @@
       <c r="Y59" s="15"/>
       <c r="Z59" s="15"/>
     </row>
-    <row r="60" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="10"/>
       <c r="B60" s="10" t="s">
         <v>20</v>
@@ -8282,7 +8291,7 @@
       </c>
       <c r="H60" s="10"/>
       <c r="I60" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J60" s="10"/>
       <c r="K60" s="10"/>
@@ -8302,7 +8311,7 @@
       <c r="Y60" s="15"/>
       <c r="Z60" s="15"/>
     </row>
-    <row r="61" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="10" t="s">
         <v>20</v>
@@ -8339,7 +8348,7 @@
       <c r="Y61" s="15"/>
       <c r="Z61" s="15"/>
     </row>
-    <row r="62" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="10" t="s">
         <v>20</v>
@@ -8378,7 +8387,7 @@
       <c r="Y62" s="15"/>
       <c r="Z62" s="15"/>
     </row>
-    <row r="63" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="10" t="s">
         <v>20</v>
@@ -8397,7 +8406,7 @@
       </c>
       <c r="H63" s="10"/>
       <c r="I63" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J63" s="10"/>
       <c r="K63" s="10"/>
@@ -8417,7 +8426,7 @@
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
     </row>
-    <row r="64" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="10"/>
       <c r="B64" s="10" t="s">
         <v>20</v>
@@ -8436,7 +8445,7 @@
       </c>
       <c r="H64" s="10"/>
       <c r="I64" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J64" s="10"/>
       <c r="K64" s="10"/>
@@ -8456,7 +8465,7 @@
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
     </row>
-    <row r="65" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="10"/>
       <c r="B65" s="10" t="s">
         <v>20</v>
@@ -8493,7 +8502,7 @@
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
     </row>
-    <row r="66" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10"/>
       <c r="B66" s="10" t="s">
         <v>20</v>
@@ -8532,7 +8541,7 @@
       <c r="Y66" s="15"/>
       <c r="Z66" s="15"/>
     </row>
-    <row r="67" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10"/>
       <c r="B67" s="10" t="s">
         <v>20</v>
@@ -8551,7 +8560,7 @@
       </c>
       <c r="H67" s="10"/>
       <c r="I67" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J67" s="10"/>
       <c r="K67" s="10"/>
@@ -8571,14 +8580,14 @@
       <c r="Y67" s="15"/>
       <c r="Z67" s="15"/>
     </row>
-    <row r="68" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10"/>
       <c r="B68" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E68" s="10" t="str">
         <f t="shared" ref="E68" si="10">LOWER(SUBSTITUTE(D68," ","_"))</f>
@@ -8590,7 +8599,7 @@
       </c>
       <c r="H68" s="10"/>
       <c r="I68" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J68" s="10"/>
       <c r="K68" s="10"/>
@@ -8610,7 +8619,7 @@
       <c r="Y68" s="15"/>
       <c r="Z68" s="15"/>
     </row>
-    <row r="69" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10"/>
       <c r="B69" s="10" t="s">
         <v>20</v>
@@ -8647,7 +8656,7 @@
       <c r="Y69" s="15"/>
       <c r="Z69" s="15"/>
     </row>
-    <row r="70" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="10"/>
       <c r="B70" s="10" t="s">
         <v>20</v>
@@ -8686,14 +8695,14 @@
       <c r="Y70" s="15"/>
       <c r="Z70" s="15"/>
     </row>
-    <row r="71" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="10"/>
       <c r="B71" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E71" s="10" t="str">
         <f t="shared" ref="E71:E74" si="11">LOWER(SUBSTITUTE(D71," ","_"))</f>
@@ -8705,7 +8714,7 @@
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
@@ -8725,14 +8734,14 @@
       <c r="Y71" s="15"/>
       <c r="Z71" s="15"/>
     </row>
-    <row r="72" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="10"/>
       <c r="B72" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E72" s="10" t="str">
         <f t="shared" si="11"/>
@@ -8744,7 +8753,7 @@
       </c>
       <c r="H72" s="10"/>
       <c r="I72" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J72" s="10"/>
       <c r="K72" s="10"/>
@@ -8764,14 +8773,14 @@
       <c r="Y72" s="15"/>
       <c r="Z72" s="15"/>
     </row>
-    <row r="73" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="10"/>
       <c r="B73" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E73" s="10" t="str">
         <f t="shared" si="11"/>
@@ -8801,14 +8810,14 @@
       <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
     </row>
-    <row r="74" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10"/>
       <c r="B74" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C74" s="10"/>
       <c r="D74" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E74" s="10" t="str">
         <f t="shared" si="11"/>
@@ -8845,7 +8854,7 @@
         <v>1</v>
       </c>
       <c r="B75" s="48" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C75" s="48" t="s">
         <v>269</v>
@@ -8912,7 +8921,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="77" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="10"/>
       <c r="B77" s="10" t="s">
         <v>20</v>
@@ -8931,7 +8940,7 @@
       </c>
       <c r="H77" s="10"/>
       <c r="I77" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J77" s="10"/>
       <c r="K77" s="10"/>
@@ -8951,7 +8960,7 @@
       <c r="Y77" s="15"/>
       <c r="Z77" s="15"/>
     </row>
-    <row r="78" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="10"/>
       <c r="B78" s="10" t="s">
         <v>20</v>
@@ -8970,7 +8979,7 @@
       </c>
       <c r="H78" s="10"/>
       <c r="I78" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J78" s="10"/>
       <c r="K78" s="10"/>
@@ -8990,7 +8999,7 @@
       <c r="Y78" s="15"/>
       <c r="Z78" s="15"/>
     </row>
-    <row r="79" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="10"/>
       <c r="B79" s="10" t="s">
         <v>20</v>
@@ -9008,7 +9017,9 @@
         <v>169</v>
       </c>
       <c r="H79" s="10"/>
-      <c r="I79" s="51"/>
+      <c r="I79" s="51">
+        <v>959</v>
+      </c>
       <c r="J79" s="10"/>
       <c r="K79" s="10"/>
       <c r="L79" s="10"/>
@@ -9027,7 +9038,7 @@
       <c r="Y79" s="15"/>
       <c r="Z79" s="15"/>
     </row>
-    <row r="80" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="10"/>
       <c r="B80" s="10" t="s">
         <v>20</v>
@@ -9046,7 +9057,7 @@
       </c>
       <c r="H80" s="10"/>
       <c r="I80" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J80" s="10"/>
       <c r="K80" s="10"/>
@@ -9066,7 +9077,7 @@
       <c r="Y80" s="15"/>
       <c r="Z80" s="15"/>
     </row>
-    <row r="81" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="10"/>
       <c r="B81" s="10" t="s">
         <v>20</v>
@@ -9085,7 +9096,7 @@
       </c>
       <c r="H81" s="10"/>
       <c r="I81" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J81" s="10"/>
       <c r="K81" s="10"/>
@@ -9105,7 +9116,7 @@
       <c r="Y81" s="15"/>
       <c r="Z81" s="15"/>
     </row>
-    <row r="82" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="10"/>
       <c r="B82" s="10" t="s">
         <v>20</v>
@@ -9124,7 +9135,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="I82" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J82" s="10"/>
       <c r="K82" s="10"/>
@@ -9144,7 +9155,7 @@
       <c r="Y82" s="15"/>
       <c r="Z82" s="15"/>
     </row>
-    <row r="83" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="10" t="s">
         <v>20</v>
@@ -9162,7 +9173,9 @@
         <v>169</v>
       </c>
       <c r="H83" s="10"/>
-      <c r="I83" s="51"/>
+      <c r="I83" s="51">
+        <v>959</v>
+      </c>
       <c r="J83" s="10"/>
       <c r="K83" s="10"/>
       <c r="L83" s="10"/>
@@ -9181,7 +9194,7 @@
       <c r="Y83" s="15"/>
       <c r="Z83" s="15"/>
     </row>
-    <row r="84" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="10"/>
       <c r="B84" s="10" t="s">
         <v>20</v>
@@ -9200,7 +9213,7 @@
       </c>
       <c r="H84" s="10"/>
       <c r="I84" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J84" s="10"/>
       <c r="K84" s="10"/>
@@ -9220,7 +9233,7 @@
       <c r="Y84" s="15"/>
       <c r="Z84" s="15"/>
     </row>
-    <row r="85" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="10" t="s">
         <v>20</v>
@@ -9239,7 +9252,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="I85" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J85" s="10"/>
       <c r="K85" s="10"/>
@@ -9259,14 +9272,14 @@
       <c r="Y85" s="15"/>
       <c r="Z85" s="15"/>
     </row>
-    <row r="86" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="10"/>
       <c r="B86" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C86" s="10"/>
       <c r="D86" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E86" s="10" t="str">
         <f t="shared" si="12"/>
@@ -9278,7 +9291,7 @@
       </c>
       <c r="H86" s="10"/>
       <c r="I86" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J86" s="10"/>
       <c r="K86" s="10"/>
@@ -9298,7 +9311,7 @@
       <c r="Y86" s="15"/>
       <c r="Z86" s="15"/>
     </row>
-    <row r="87" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="10"/>
       <c r="B87" s="10" t="s">
         <v>20</v>
@@ -9316,7 +9329,9 @@
         <v>169</v>
       </c>
       <c r="H87" s="10"/>
-      <c r="I87" s="51"/>
+      <c r="I87" s="51">
+        <v>959</v>
+      </c>
       <c r="J87" s="10"/>
       <c r="K87" s="10"/>
       <c r="L87" s="10"/>
@@ -9335,7 +9350,7 @@
       <c r="Y87" s="15"/>
       <c r="Z87" s="15"/>
     </row>
-    <row r="88" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="10"/>
       <c r="B88" s="10" t="s">
         <v>20</v>
@@ -9354,7 +9369,7 @@
       </c>
       <c r="H88" s="10"/>
       <c r="I88" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J88" s="10"/>
       <c r="K88" s="10"/>
@@ -9379,7 +9394,7 @@
         <v>1</v>
       </c>
       <c r="B89" s="48" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C89" s="48" t="s">
         <v>269</v>
@@ -9446,7 +9461,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="91" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="10"/>
       <c r="B91" s="10" t="s">
         <v>20</v>
@@ -9465,7 +9480,7 @@
       </c>
       <c r="H91" s="10"/>
       <c r="I91" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J91" s="10"/>
       <c r="K91" s="10"/>
@@ -9485,7 +9500,7 @@
       <c r="Y91" s="15"/>
       <c r="Z91" s="15"/>
     </row>
-    <row r="92" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="10"/>
       <c r="B92" s="10" t="s">
         <v>20</v>
@@ -9504,7 +9519,7 @@
       </c>
       <c r="H92" s="10"/>
       <c r="I92" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J92" s="10"/>
       <c r="K92" s="10"/>
@@ -9524,7 +9539,7 @@
       <c r="Y92" s="15"/>
       <c r="Z92" s="15"/>
     </row>
-    <row r="93" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="10"/>
       <c r="B93" s="10" t="s">
         <v>20</v>
@@ -9542,7 +9557,9 @@
         <v>169</v>
       </c>
       <c r="H93" s="10"/>
-      <c r="I93" s="51"/>
+      <c r="I93" s="51">
+        <v>662</v>
+      </c>
       <c r="J93" s="10"/>
       <c r="K93" s="10"/>
       <c r="L93" s="10"/>
@@ -9561,7 +9578,7 @@
       <c r="Y93" s="15"/>
       <c r="Z93" s="15"/>
     </row>
-    <row r="94" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10"/>
       <c r="B94" s="10" t="s">
         <v>20</v>
@@ -9580,7 +9597,7 @@
       </c>
       <c r="H94" s="10"/>
       <c r="I94" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J94" s="10"/>
       <c r="K94" s="10"/>
@@ -9600,7 +9617,7 @@
       <c r="Y94" s="15"/>
       <c r="Z94" s="15"/>
     </row>
-    <row r="95" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10"/>
       <c r="B95" s="10" t="s">
         <v>20</v>
@@ -9619,7 +9636,7 @@
       </c>
       <c r="H95" s="10"/>
       <c r="I95" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J95" s="10"/>
       <c r="K95" s="10"/>
@@ -9639,7 +9656,7 @@
       <c r="Y95" s="15"/>
       <c r="Z95" s="15"/>
     </row>
-    <row r="96" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10"/>
       <c r="B96" s="10" t="s">
         <v>20</v>
@@ -9658,7 +9675,7 @@
       </c>
       <c r="H96" s="10"/>
       <c r="I96" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J96" s="10"/>
       <c r="K96" s="10"/>
@@ -9678,7 +9695,7 @@
       <c r="Y96" s="15"/>
       <c r="Z96" s="15"/>
     </row>
-    <row r="97" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10"/>
       <c r="B97" s="10" t="s">
         <v>20</v>
@@ -9696,7 +9713,9 @@
         <v>169</v>
       </c>
       <c r="H97" s="10"/>
-      <c r="I97" s="51"/>
+      <c r="I97" s="51">
+        <v>662</v>
+      </c>
       <c r="J97" s="10"/>
       <c r="K97" s="10"/>
       <c r="L97" s="10"/>
@@ -9715,7 +9734,7 @@
       <c r="Y97" s="15"/>
       <c r="Z97" s="15"/>
     </row>
-    <row r="98" spans="1:26" s="54" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" s="53" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10"/>
       <c r="B98" s="10" t="s">
         <v>20</v>
@@ -9734,7 +9753,7 @@
       </c>
       <c r="H98" s="10"/>
       <c r="I98" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J98" s="10"/>
       <c r="K98" s="10"/>
@@ -9754,7 +9773,7 @@
       <c r="Y98" s="15"/>
       <c r="Z98" s="15"/>
     </row>
-    <row r="99" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10"/>
       <c r="B99" s="10" t="s">
         <v>20</v>
@@ -9773,7 +9792,7 @@
       </c>
       <c r="H99" s="10"/>
       <c r="I99" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J99" s="10"/>
       <c r="K99" s="10"/>
@@ -9793,14 +9812,14 @@
       <c r="Y99" s="15"/>
       <c r="Z99" s="15"/>
     </row>
-    <row r="100" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10"/>
       <c r="B100" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E100" s="10" t="str">
         <f t="shared" si="13"/>
@@ -9812,7 +9831,7 @@
       </c>
       <c r="H100" s="10"/>
       <c r="I100" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J100" s="10"/>
       <c r="K100" s="10"/>
@@ -9832,7 +9851,7 @@
       <c r="Y100" s="15"/>
       <c r="Z100" s="15"/>
     </row>
-    <row r="101" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10"/>
       <c r="B101" s="10" t="s">
         <v>20</v>
@@ -9850,7 +9869,9 @@
         <v>169</v>
       </c>
       <c r="H101" s="10"/>
-      <c r="I101" s="51"/>
+      <c r="I101" s="51">
+        <v>662</v>
+      </c>
       <c r="J101" s="10"/>
       <c r="K101" s="10"/>
       <c r="L101" s="10"/>
@@ -9869,7 +9890,7 @@
       <c r="Y101" s="15"/>
       <c r="Z101" s="15"/>
     </row>
-    <row r="102" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="10"/>
       <c r="B102" s="10" t="s">
         <v>20</v>
@@ -9888,7 +9909,7 @@
       </c>
       <c r="H102" s="10"/>
       <c r="I102" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J102" s="10"/>
       <c r="K102" s="10"/>
@@ -9913,7 +9934,7 @@
         <v>1</v>
       </c>
       <c r="B103" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C103" s="48" t="s">
         <v>269</v>
@@ -9999,7 +10020,7 @@
       </c>
       <c r="H105" s="10"/>
       <c r="I105" s="21" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J105" s="10"/>
       <c r="K105" s="10"/>
@@ -10019,7 +10040,7 @@
       <c r="Y105" s="15"/>
       <c r="Z105" s="15"/>
     </row>
-    <row r="106" spans="1:26" s="54" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="10"/>
       <c r="B106" s="10" t="s">
         <v>20</v>
@@ -10037,8 +10058,8 @@
         <v>233</v>
       </c>
       <c r="H106" s="10"/>
-      <c r="I106" s="54" t="s">
-        <v>428</v>
+      <c r="I106" s="53" t="s">
+        <v>427</v>
       </c>
       <c r="J106" s="10"/>
       <c r="K106" s="10"/>
@@ -10077,7 +10098,7 @@
       </c>
       <c r="H107" s="10"/>
       <c r="I107" s="51">
-        <v>10</v>
+        <v>629.24</v>
       </c>
       <c r="J107" s="10"/>
       <c r="K107" s="10"/>
@@ -10115,8 +10136,8 @@
         <v>233</v>
       </c>
       <c r="H108" s="10"/>
-      <c r="I108" s="54" t="s">
-        <v>439</v>
+      <c r="I108" s="53" t="s">
+        <v>438</v>
       </c>
       <c r="J108" s="10"/>
       <c r="K108" s="10"/>
@@ -10266,7 +10287,7 @@
       </c>
       <c r="H112" s="10"/>
       <c r="I112" s="51">
-        <v>0.09</v>
+        <v>0.12</v>
       </c>
       <c r="J112" s="10"/>
       <c r="K112" s="10"/>

</xml_diff>

<commit_message>
Decoding geographic fields in ahs data.
</commit_message>
<xml_diff>
--- a/projects/resstock_pnw_10_measures.xlsx
+++ b/projects/resstock_pnw_10_measures.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4515" yWindow="1125" windowWidth="20490" windowHeight="8235" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="4515" yWindow="1185" windowWidth="20490" windowHeight="8175" tabRatio="562" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -5951,9 +5951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7877,7 +7875,9 @@
         <v>169</v>
       </c>
       <c r="H49" s="10"/>
-      <c r="I49" s="51"/>
+      <c r="I49" s="51">
+        <v>10</v>
+      </c>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
       <c r="L49" s="10"/>
@@ -8103,7 +8103,9 @@
         <v>169</v>
       </c>
       <c r="H55" s="10"/>
-      <c r="I55" s="51"/>
+      <c r="I55" s="51">
+        <v>10</v>
+      </c>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
       <c r="L55" s="10"/>
@@ -8329,7 +8331,9 @@
         <v>169</v>
       </c>
       <c r="H61" s="10"/>
-      <c r="I61" s="51"/>
+      <c r="I61" s="51">
+        <v>13</v>
+      </c>
       <c r="J61" s="10"/>
       <c r="K61" s="10"/>
       <c r="L61" s="10"/>
@@ -8483,7 +8487,9 @@
         <v>169</v>
       </c>
       <c r="H65" s="10"/>
-      <c r="I65" s="51"/>
+      <c r="I65" s="51">
+        <v>13</v>
+      </c>
       <c r="J65" s="10"/>
       <c r="K65" s="10"/>
       <c r="L65" s="10"/>
@@ -8637,7 +8643,9 @@
         <v>169</v>
       </c>
       <c r="H69" s="10"/>
-      <c r="I69" s="51"/>
+      <c r="I69" s="51">
+        <v>13</v>
+      </c>
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
       <c r="L69" s="10"/>
@@ -8791,7 +8799,9 @@
         <v>169</v>
       </c>
       <c r="H73" s="10"/>
-      <c r="I73" s="51"/>
+      <c r="I73" s="51">
+        <v>13</v>
+      </c>
       <c r="J73" s="10"/>
       <c r="K73" s="10"/>
       <c r="L73" s="10"/>

</xml_diff>